<commit_message>
graficos tiempo de solucion
</commit_message>
<xml_diff>
--- a/soluciones_ejemplos.xlsx
+++ b/soluciones_ejemplos.xlsx
@@ -105,7 +105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +116,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -152,10 +158,10 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -480,7 +486,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +494,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -496,7 +502,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -504,7 +510,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -512,7 +518,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -520,7 +526,7 @@
         <v>1682</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -528,7 +534,7 @@
         <v>2144</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -536,7 +542,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -544,7 +550,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -552,7 +558,7 @@
         <v>10627</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -560,7 +566,7 @@
         <v>11741</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -568,7 +574,7 @@
         <v>17573</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -576,7 +582,7 @@
         <v>14420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -584,7 +590,7 @@
         <v>15126</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -592,7 +598,7 @@
         <v>14976</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -600,7 +606,7 @@
         <v>17170</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -608,7 +614,7 @@
         <v>18367</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -616,7 +622,7 @@
         <v>14965</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -624,7 +630,7 @@
         <v>18989</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -632,7 +638,7 @@
         <v>16764</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -640,7 +646,7 @@
         <v>18819</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -648,7 +654,7 @@
         <v>20960</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -656,7 +662,7 @@
         <v>19185</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -664,7 +670,7 @@
         <v>18807</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -672,7 +678,7 @@
         <v>23926</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -680,7 +686,7 @@
         <v>13331</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -688,7 +694,7 @@
         <v>19339</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -696,7 +702,7 @@
         <v>22744</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>